<commit_message>
Forgot to commit earlier. Now starting development on Input handeling.
</commit_message>
<xml_diff>
--- a/PauseTexts.xlsx
+++ b/PauseTexts.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{127DB198-D237-423D-AAFD-DB53E95E136D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{52E75E68-1054-4489-8968-E9BD9B77C681}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Randoms</t>
   </si>
@@ -86,6 +86,15 @@
   </si>
   <si>
     <t>Addictive thoughts</t>
+  </si>
+  <si>
+    <t>followup</t>
+  </si>
+  <si>
+    <t>After pain comes satisfaction</t>
+  </si>
+  <si>
+    <t>Always.</t>
   </si>
 </sst>
 </file>
@@ -127,12 +136,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -410,106 +420,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:I13"/>
+  <dimension ref="A3:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="36.5703125" customWidth="1"/>
-    <col min="5" max="5" width="36.5703125" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" customWidth="1"/>
+    <col min="3" max="4" width="36.5703125" customWidth="1"/>
+    <col min="6" max="6" width="36.5703125" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
         <v>3</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>4</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>2</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E10" t="s">
+      <c r="D10" s="2"/>
+      <c r="F10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>14</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Level generation is now somewhat useable
</commit_message>
<xml_diff>
--- a/PauseTexts.xlsx
+++ b/PauseTexts.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5F80B06E-0CFB-48AB-BE8D-479F1E68AC28}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{84B9949C-E1BB-40F9-917C-5D95D946DDC8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Randoms</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t>For death and glory</t>
+  </si>
+  <si>
+    <t>Fish can roll</t>
+  </si>
+  <si>
+    <t>Dead man walkin'</t>
   </si>
 </sst>
 </file>
@@ -435,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:J16"/>
+  <dimension ref="A3:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,6 +574,16 @@
         <v>27</v>
       </c>
     </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>